<commit_message>
updates to index and others
</commit_message>
<xml_diff>
--- a/CodeSystem-airport-code-system.xlsx
+++ b/CodeSystem-airport-code-system.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="138">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-12-11T14:30:36-05:00</t>
+    <t>2024-01-05T10:12:51-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -111,7 +111,7 @@
     <t>Count</t>
   </si>
   <si>
-    <t>4</t>
+    <t>52</t>
   </si>
   <si>
     <t>Level</t>
@@ -147,10 +147,286 @@
     <t>Los Angeles, CA</t>
   </si>
   <si>
+    <t>MIA</t>
+  </si>
+  <si>
+    <t>Miami, FL</t>
+  </si>
+  <si>
+    <t>ATL</t>
+  </si>
+  <si>
+    <t>Atlanta, GA</t>
+  </si>
+  <si>
+    <t>ORD</t>
+  </si>
+  <si>
+    <t>Chicago, IL</t>
+  </si>
+  <si>
+    <t>DFW</t>
+  </si>
+  <si>
+    <t>Dallas/Fort Worth, TX</t>
+  </si>
+  <si>
+    <t>DEN</t>
+  </si>
+  <si>
+    <t>Denver, CO</t>
+  </si>
+  <si>
+    <t>JFK</t>
+  </si>
+  <si>
+    <t>New York, NY</t>
+  </si>
+  <si>
+    <t>SFO</t>
+  </si>
+  <si>
+    <t>San Francisco, CA</t>
+  </si>
+  <si>
+    <t>SEA</t>
+  </si>
+  <si>
+    <t>Seattle, WA</t>
+  </si>
+  <si>
+    <t>LAS</t>
+  </si>
+  <si>
+    <t>Las Vegas, NV</t>
+  </si>
+  <si>
+    <t>PHX</t>
+  </si>
+  <si>
+    <t>Phoenix, AZ</t>
+  </si>
+  <si>
+    <t>MSP</t>
+  </si>
+  <si>
+    <t>Minneapolis, MN</t>
+  </si>
+  <si>
+    <t>DTW</t>
+  </si>
+  <si>
+    <t>Detroit, MI</t>
+  </si>
+  <si>
+    <t>PHL</t>
+  </si>
+  <si>
+    <t>Philadelphia, PA</t>
+  </si>
+  <si>
+    <t>BOS</t>
+  </si>
+  <si>
+    <t>Boston, MA</t>
+  </si>
+  <si>
+    <t>LGA</t>
+  </si>
+  <si>
+    <t>EWR</t>
+  </si>
+  <si>
+    <t>Newark, NJ</t>
+  </si>
+  <si>
+    <t>CLT</t>
+  </si>
+  <si>
+    <t>Charlotte, NC</t>
+  </si>
+  <si>
+    <t>IAH</t>
+  </si>
+  <si>
+    <t>Houston, TX</t>
+  </si>
+  <si>
     <t>DCA</t>
   </si>
   <si>
     <t>Washington, DC</t>
+  </si>
+  <si>
+    <t>FLL</t>
+  </si>
+  <si>
+    <t>Fort Lauderdale, FL</t>
+  </si>
+  <si>
+    <t>MDW</t>
+  </si>
+  <si>
+    <t>SAN</t>
+  </si>
+  <si>
+    <t>San Diego, CA</t>
+  </si>
+  <si>
+    <t>TPA</t>
+  </si>
+  <si>
+    <t>Tampa, FL</t>
+  </si>
+  <si>
+    <t>HNL</t>
+  </si>
+  <si>
+    <t>Honolulu, HI</t>
+  </si>
+  <si>
+    <t>PDX</t>
+  </si>
+  <si>
+    <t>Portland, OR</t>
+  </si>
+  <si>
+    <t>STL</t>
+  </si>
+  <si>
+    <t>St. Louis, MO</t>
+  </si>
+  <si>
+    <t>MCO</t>
+  </si>
+  <si>
+    <t>Orlando, FL</t>
+  </si>
+  <si>
+    <t>BWI</t>
+  </si>
+  <si>
+    <t>Baltimore, MD</t>
+  </si>
+  <si>
+    <t>SLC</t>
+  </si>
+  <si>
+    <t>Salt Lake City, UT</t>
+  </si>
+  <si>
+    <t>IAD</t>
+  </si>
+  <si>
+    <t>AUS</t>
+  </si>
+  <si>
+    <t>Austin, TX</t>
+  </si>
+  <si>
+    <t>SJC</t>
+  </si>
+  <si>
+    <t>San Jose, CA</t>
+  </si>
+  <si>
+    <t>DAL</t>
+  </si>
+  <si>
+    <t>Dallas, TX</t>
+  </si>
+  <si>
+    <t>HOU</t>
+  </si>
+  <si>
+    <t>RDU</t>
+  </si>
+  <si>
+    <t>Raleigh/Durham, NC</t>
+  </si>
+  <si>
+    <t>BNA</t>
+  </si>
+  <si>
+    <t>Nashville, TN</t>
+  </si>
+  <si>
+    <t>MSY</t>
+  </si>
+  <si>
+    <t>New Orleans, LA</t>
+  </si>
+  <si>
+    <t>SMF</t>
+  </si>
+  <si>
+    <t>Sacramento, CA</t>
+  </si>
+  <si>
+    <t>IND</t>
+  </si>
+  <si>
+    <t>Indianapolis, IN</t>
+  </si>
+  <si>
+    <t>MKE</t>
+  </si>
+  <si>
+    <t>Milwaukee, WI</t>
+  </si>
+  <si>
+    <t>JAX</t>
+  </si>
+  <si>
+    <t>Jacksonville, FL</t>
+  </si>
+  <si>
+    <t>SAT</t>
+  </si>
+  <si>
+    <t>San Antonio, TX</t>
+  </si>
+  <si>
+    <t>PIT</t>
+  </si>
+  <si>
+    <t>Pittsburgh, PA</t>
+  </si>
+  <si>
+    <t>SNA</t>
+  </si>
+  <si>
+    <t>Santa Ana, CA</t>
+  </si>
+  <si>
+    <t>RSW</t>
+  </si>
+  <si>
+    <t>Fort Myers, FL</t>
+  </si>
+  <si>
+    <t>CLE</t>
+  </si>
+  <si>
+    <t>Cleveland, OH</t>
+  </si>
+  <si>
+    <t>CMH</t>
+  </si>
+  <si>
+    <t>Columbus, OH</t>
+  </si>
+  <si>
+    <t>OGG</t>
+  </si>
+  <si>
+    <t>Kahului, HI</t>
+  </si>
+  <si>
+    <t>PBI</t>
+  </si>
+  <si>
+    <t>West Palm Beach, FL</t>
   </si>
 </sst>
 </file>
@@ -451,7 +727,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -519,6 +795,582 @@
       </c>
       <c r="D5" s="2"/>
     </row>
+    <row r="6">
+      <c r="A6" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="C12" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="C13" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="C14" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="C15" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="C17" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="C18" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="C19" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="C20" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B21" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="C21" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="C22" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B23" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="C23" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="C24" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B25" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="C25" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B26" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="C26" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B27" t="s" s="2">
+        <v>86</v>
+      </c>
+      <c r="C27" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B28" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="C28" t="s" s="2">
+        <v>89</v>
+      </c>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B29" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="C29" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B30" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="C30" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B31" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="C31" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B32" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="C32" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B33" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="C33" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B34" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="C34" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B35" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="C35" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B36" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="C36" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="C37" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="C38" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s" s="2">
+        <v>108</v>
+      </c>
+      <c r="C39" t="s" s="2">
+        <v>109</v>
+      </c>
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B40" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="C40" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B41" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="C41" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B42" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="C42" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B43" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="C43" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B44" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="C44" t="s" s="2">
+        <v>119</v>
+      </c>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B45" t="s" s="2">
+        <v>120</v>
+      </c>
+      <c r="C45" t="s" s="2">
+        <v>121</v>
+      </c>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B46" t="s" s="2">
+        <v>122</v>
+      </c>
+      <c r="C46" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B47" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="C47" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B48" t="s" s="2">
+        <v>126</v>
+      </c>
+      <c r="C48" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B49" t="s" s="2">
+        <v>128</v>
+      </c>
+      <c r="C49" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B50" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="C50" t="s" s="2">
+        <v>131</v>
+      </c>
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B51" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="C51" t="s" s="2">
+        <v>133</v>
+      </c>
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B52" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="C52" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B53" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="C53" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="D53" s="2"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>